<commit_message>
Fixed chart 7, 12, 13, 14
</commit_message>
<xml_diff>
--- a/docs/blanksheet.xlsx
+++ b/docs/blanksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abiyyu\Desktop\programming\dashboard-mock\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D019221-2A19-4512-9AA4-82EA36A50F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEFAB5D-DF38-4A77-8B50-53C4CCF039E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{A374144C-A715-4AA7-9BB0-AB25833D26FF}"/>
   </bookViews>
@@ -36,51 +36,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>tahun</t>
+  </si>
+  <si>
+    <t>kabupaten</t>
+  </si>
+  <si>
+    <t>provinsi</t>
+  </si>
+  <si>
+    <t>jenis_kendaraan</t>
+  </si>
+  <si>
+    <t>jumlah_kendaraan</t>
+  </si>
+  <si>
+    <t>jumlah_kendaraan_bayar</t>
+  </si>
+  <si>
+    <t>jumlah_pembayaran_online</t>
+  </si>
+  <si>
+    <t>jumlah_pembayaran_offline</t>
+  </si>
+  <si>
+    <t>nominal_menunggak_1tahun</t>
+  </si>
+  <si>
+    <t>nominal_menunggak_5tahun</t>
+  </si>
+  <si>
+    <t>nominal_menunggak_7tahun</t>
+  </si>
+  <si>
+    <t>jumlah_menunggak_5tahun</t>
+  </si>
+  <si>
+    <t>nominal_pembayaran_online</t>
+  </si>
+  <si>
+    <t>nominal_pembayaran_offline</t>
+  </si>
+  <si>
+    <t>jenis_kepemilikan</t>
+  </si>
   <si>
     <t>bulan</t>
-  </si>
-  <si>
-    <t>tahun</t>
-  </si>
-  <si>
-    <t>kabupaten</t>
-  </si>
-  <si>
-    <t>provinsi</t>
-  </si>
-  <si>
-    <t>jenis_kendaraan</t>
-  </si>
-  <si>
-    <t>jumlah_kendaraan</t>
-  </si>
-  <si>
-    <t>jumlah_kendaraan_bayar</t>
-  </si>
-  <si>
-    <t>jumlah_pembayaran_online</t>
-  </si>
-  <si>
-    <t>nilai_pembayaran_online</t>
-  </si>
-  <si>
-    <t>nilai_pembayaran_offline</t>
-  </si>
-  <si>
-    <t>jumlah_pembayaran_offline</t>
-  </si>
-  <si>
-    <t>nominal_menunggak_1tahun</t>
-  </si>
-  <si>
-    <t>nominal_menunggak_5tahun</t>
-  </si>
-  <si>
-    <t>nominal_menunggak_7tahun</t>
-  </si>
-  <si>
-    <t>jumlah_menunggak_5tahun</t>
   </si>
 </sst>
 </file>
@@ -461,111 +464,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EDE5A6F-D963-469E-B5D5-4D6215EB864A}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="4" width="5.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>